<commit_message>
Uploading the updated Project Test Scenario sheet and Pdf and also Test Case sheet and Pdf.
</commit_message>
<xml_diff>
--- a/Project -1 (Level-Basic)/Test Scenarios.xlsx
+++ b/Project -1 (Level-Basic)/Test Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d09b73bd954f8bef/Desktop/Manual-Testing-Projects/Project -1 (Level-Basic)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="323" documentId="8_{4A70E22D-039B-45FB-98EE-ABEF17ECCA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4FCDB5C-0075-42A2-8BCA-0587A9672757}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{4A70E22D-039B-45FB-98EE-ABEF17ECCA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{547F3CED-4770-4B16-B8BF-886A8E47AE37}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3EED3199-83E8-4D4E-A02F-FC69AD882DE0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>Project Name:</t>
   </si>
@@ -78,15 +78,6 @@
     <t>Excepted Result</t>
   </si>
   <si>
-    <t>Actual Result</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>TS_01</t>
   </si>
   <si>
@@ -102,12 +93,6 @@
     <t>1.User click the registration button.</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
-    <t>Registration page load checking</t>
-  </si>
-  <si>
     <t>TS_02</t>
   </si>
   <si>
@@ -124,9 +109,6 @@
   </si>
   <si>
     <t>Verify all input fields will be properly display</t>
-  </si>
-  <si>
-    <t>Registartion page input fields checking</t>
   </si>
   <si>
     <t>TS_03</t>
@@ -143,9 +125,6 @@
   </si>
   <si>
     <t>All the input fields should be accessible for data entry</t>
-  </si>
-  <si>
-    <t>Input fields checking</t>
   </si>
   <si>
     <t>TS_04</t>
@@ -162,9 +141,6 @@
     <t>No any effect on user registration by filling and filling the optional input fields</t>
   </si>
   <si>
-    <t>Ensuring optional fields will work properly</t>
-  </si>
-  <si>
     <t>TS_05</t>
   </si>
   <si>
@@ -182,9 +158,6 @@
     <t>Registration will not be successful and mandatory field must be filled as message will be pop-up</t>
   </si>
   <si>
-    <t>Ensuring that mandatory fields work propely</t>
-  </si>
-  <si>
     <t>TS_06</t>
   </si>
   <si>
@@ -198,9 +171,6 @@
     <t>Only one option can be click at one time</t>
   </si>
   <si>
-    <t>Checking the Gender input</t>
-  </si>
-  <si>
     <t>TS_07</t>
   </si>
   <si>
@@ -214,9 +184,6 @@
     <t>Registration will be successful in case of alphabetical characters in First Name input</t>
   </si>
   <si>
-    <t>First Name input checking</t>
-  </si>
-  <si>
     <t>TS_08</t>
   </si>
   <si>
@@ -230,9 +197,6 @@
     <t>Registration will be successful in case of alphabetical characters in Last Name input</t>
   </si>
   <si>
-    <t>Last Name input checking</t>
-  </si>
-  <si>
     <t>TS_09</t>
   </si>
   <si>
@@ -246,9 +210,6 @@
     <t>Accept only unique and correct email id</t>
   </si>
   <si>
-    <t>Email id input checking</t>
-  </si>
-  <si>
     <t>TS_10</t>
   </si>
   <si>
@@ -262,9 +223,6 @@
     <t>Default checked and can be edited</t>
   </si>
   <si>
-    <t>Newsletter checking</t>
-  </si>
-  <si>
     <t>TS_11</t>
   </si>
   <si>
@@ -276,9 +234,6 @@
   </si>
   <si>
     <t>Auto-suggest strong password and should be accept 6-16 length of password with upercase,lowercase,numeric and special characters</t>
-  </si>
-  <si>
-    <t>Password input field checking</t>
   </si>
   <si>
     <t>TS_12</t>
@@ -293,9 +248,6 @@
   </si>
   <si>
     <t>Confirm Password must be matched with Password in unmatched case error message will be appear</t>
-  </si>
-  <si>
-    <t>Confirm password input checking</t>
   </si>
   <si>
     <t>TS_13</t>
@@ -316,9 +268,6 @@
   </si>
   <si>
     <t>Registration successful of new user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New user registration </t>
   </si>
   <si>
     <t>TS_14</t>
@@ -338,9 +287,6 @@
   </si>
   <si>
     <t>User can login easily with their correct email id and password</t>
-  </si>
-  <si>
-    <t>Login checking</t>
   </si>
 </sst>
 </file>
@@ -392,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -436,17 +382,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -466,22 +401,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -505,9 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -518,12 +439,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -844,50 +759,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38CB621-4805-41CC-99A6-62142EC0FC84}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D3" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="172.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="56.6640625" customWidth="1"/>
-    <col min="6" max="6" width="128.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" customWidth="1"/>
-    <col min="9" max="9" width="43" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="125.6640625" customWidth="1"/>
+    <col min="4" max="4" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="128.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -895,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -903,7 +809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -911,7 +817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -919,7 +825,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -927,7 +833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -946,397 +852,290 @@
       <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="5" t="s">
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="F11" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="B12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="6" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="6" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="F15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="D17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="6" t="s">
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="6" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="B19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="7" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="B20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="D20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="F20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="B21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="D21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="6" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="B23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="6" t="s">
+    </row>
+    <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="B24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F24" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Uploading the updated and correct Test Scenario sheet and Pdf.
</commit_message>
<xml_diff>
--- a/Project -1 (Level-Basic)/Test Scenarios.xlsx
+++ b/Project -1 (Level-Basic)/Test Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d09b73bd954f8bef/Desktop/Manual-Testing-Projects/Project -1 (Level-Basic)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="337" documentId="8_{4A70E22D-039B-45FB-98EE-ABEF17ECCA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{547F3CED-4770-4B16-B8BF-886A8E47AE37}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="8_{4A70E22D-039B-45FB-98EE-ABEF17ECCA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4C98BEA-6B27-43E9-B3B7-4BB969DAFA06}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3EED3199-83E8-4D4E-A02F-FC69AD882DE0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Project Name:</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Test Steps</t>
   </si>
   <si>
-    <t>Excepted Result</t>
-  </si>
-  <si>
     <t>TS_01</t>
   </si>
   <si>
@@ -96,16 +93,10 @@
     <t>TS_02</t>
   </si>
   <si>
-    <t>User's registration page should load with all inputs field</t>
-  </si>
-  <si>
     <t>User is on registration page</t>
   </si>
   <si>
     <t>1.Open the registration page</t>
-  </si>
-  <si>
-    <t>All input fields should be properly visible to user</t>
   </si>
   <si>
     <t>Verify all input fields will be properly display</t>
@@ -122,9 +113,6 @@
   </si>
   <si>
     <t>Test Scenario Document For Register Page Module (nopcommerce demo)</t>
-  </si>
-  <si>
-    <t>All the input fields should be accessible for data entry</t>
   </si>
   <si>
     <t>TS_04</t>
@@ -138,9 +126,6 @@
 3.Done registration of user without filling optional fields</t>
   </si>
   <si>
-    <t>No any effect on user registration by filling and filling the optional input fields</t>
-  </si>
-  <si>
     <t>TS_05</t>
   </si>
   <si>
@@ -155,9 +140,6 @@
 3.Done registration of user without filling mandatory fields</t>
   </si>
   <si>
-    <t>Registration will not be successful and mandatory field must be filled as message will be pop-up</t>
-  </si>
-  <si>
     <t>TS_06</t>
   </si>
   <si>
@@ -168,9 +150,6 @@
 2.Click the option of Gender input</t>
   </si>
   <si>
-    <t>Only one option can be click at one time</t>
-  </si>
-  <si>
     <t>TS_07</t>
   </si>
   <si>
@@ -181,9 +160,6 @@
 2.Enter the alphabetical character in First Name input</t>
   </si>
   <si>
-    <t>Registration will be successful in case of alphabetical characters in First Name input</t>
-  </si>
-  <si>
     <t>TS_08</t>
   </si>
   <si>
@@ -194,9 +170,6 @@
 2.Enter the alphabetical character in Last Name input</t>
   </si>
   <si>
-    <t>Registration will be successful in case of alphabetical characters in Last Name input</t>
-  </si>
-  <si>
     <t>TS_09</t>
   </si>
   <si>
@@ -207,9 +180,6 @@
     <t>Verify that only proper and unique email id will be submitted(eg:"abc@gmail.com")</t>
   </si>
   <si>
-    <t>Accept only unique and correct email id</t>
-  </si>
-  <si>
     <t>TS_10</t>
   </si>
   <si>
@@ -220,9 +190,6 @@
 2.Check the Newsletter input field</t>
   </si>
   <si>
-    <t>Default checked and can be edited</t>
-  </si>
-  <si>
     <t>TS_11</t>
   </si>
   <si>
@@ -231,9 +198,6 @@
   <si>
     <t>1.Open the registration page
 2.Access the Password input field</t>
-  </si>
-  <si>
-    <t>Auto-suggest strong password and should be accept 6-16 length of password with upercase,lowercase,numeric and special characters</t>
   </si>
   <si>
     <t>TS_12</t>
@@ -245,9 +209,6 @@
     <t>1.Open the registration page
 2.Filled the password field
 3.Filling same password in Confiem Password input field</t>
-  </si>
-  <si>
-    <t>Confirm Password must be matched with Password in unmatched case error message will be appear</t>
   </si>
   <si>
     <t>TS_13</t>
@@ -265,9 +226,6 @@
     <t>1.Open the registration page
 2.Fill all the mandatory input fields with unique Email id
 3.Fill properly matched Password and Confirm password</t>
-  </si>
-  <si>
-    <t>Registration successful of new user</t>
   </si>
   <si>
     <t>TS_14</t>
@@ -284,9 +242,6 @@
 3.Fill properly matched Password and Confirm password
 4.Done registration successful of new user
 5.Visit the login page and entered correct email id and password</t>
-  </si>
-  <si>
-    <t>User can login easily with their correct email id and password</t>
   </si>
 </sst>
 </file>
@@ -759,41 +714,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38CB621-4805-41CC-99A6-62142EC0FC84}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D3" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScale="43" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="125.6640625" customWidth="1"/>
-    <col min="4" max="4" width="46.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="128.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="176.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -801,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -809,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -817,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -825,7 +777,7 @@
         <v>45915</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -833,7 +785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -849,293 +801,248 @@
       <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="6" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="E14" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="D17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="D18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="6" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="B19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="7" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="B20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="D20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="D21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="6" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="B23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="D23" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="6" t="s">
+    </row>
+    <row r="24" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>